<commit_message>
add scipt/data & update progress
</commit_message>
<xml_diff>
--- a/ps.xlsx
+++ b/ps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\dcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4C1EC9-0645-47D1-A2FB-839D7BE38039}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C54B67-72B2-4102-895C-DC441EF40306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -470,9 +470,7 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>21075</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -499,9 +497,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
-        <v>21030</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -516,18 +512,14 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3">
-        <v>21059</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
-        <v>21074</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -541,45 +533,35 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3">
-        <v>21061</v>
-      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3">
-        <v>21064</v>
-      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1">
-        <v>21077</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3">
-        <v>21068</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1">
-        <v>21078</v>
-      </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -593,43 +575,33 @@
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="3">
-        <v>21055</v>
-      </c>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="2">
-        <v>21079</v>
-      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="1">
-        <v>21080</v>
-      </c>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3">
-        <v>21046</v>
-      </c>
+      <c r="B21" s="3"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="3">
-        <v>21084</v>
-      </c>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -666,7 +638,7 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <v>21056</v>
+        <v>21086</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -674,9 +646,7 @@
       <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="3">
-        <v>21083</v>
-      </c>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -689,26 +659,19 @@
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B30">
-        <v>18144</v>
-      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="3">
-        <v>21081</v>
-      </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="3">
-        <v>21082</v>
-      </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="2"/>
     </row>
   </sheetData>

</xml_diff>